<commit_message>
Bug fixes to pomelo extractor and updated tracker.
</commit_message>
<xml_diff>
--- a/tracker/stats.xlsx
+++ b/tracker/stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giant\Projects\pomelo-disease-classification\tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF16D57E-4BAD-42FD-844A-2A528C59E93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2469ACC-6D06-451C-9FFF-8F1AB3FFF124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
@@ -5093,8 +5093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1562"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6296,7 +6296,7 @@
         <v>1421</v>
       </c>
       <c r="C144" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -6304,7 +6304,7 @@
         <v>1420</v>
       </c>
       <c r="C145" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
@@ -6312,7 +6312,7 @@
         <v>1419</v>
       </c>
       <c r="C146" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
@@ -6320,7 +6320,7 @@
         <v>1418</v>
       </c>
       <c r="C147" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
@@ -6328,7 +6328,7 @@
         <v>1417</v>
       </c>
       <c r="C148" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
@@ -6336,7 +6336,7 @@
         <v>1416</v>
       </c>
       <c r="C149" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -6344,7 +6344,7 @@
         <v>1415</v>
       </c>
       <c r="C150" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
@@ -6352,7 +6352,7 @@
         <v>1414</v>
       </c>
       <c r="C151" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
@@ -6360,7 +6360,7 @@
         <v>1413</v>
       </c>
       <c r="C152" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
@@ -6368,7 +6368,7 @@
         <v>1412</v>
       </c>
       <c r="C153" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
@@ -6376,7 +6376,7 @@
         <v>1411</v>
       </c>
       <c r="C154" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -6384,7 +6384,7 @@
         <v>1410</v>
       </c>
       <c r="C155" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
@@ -6392,7 +6392,7 @@
         <v>1409</v>
       </c>
       <c r="C156" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
@@ -6400,7 +6400,7 @@
         <v>1408</v>
       </c>
       <c r="C157" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
@@ -6408,7 +6408,7 @@
         <v>1407</v>
       </c>
       <c r="C158" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
@@ -6416,7 +6416,7 @@
         <v>1406</v>
       </c>
       <c r="C159" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
@@ -6424,7 +6424,7 @@
         <v>1405</v>
       </c>
       <c r="C160" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
@@ -6432,7 +6432,7 @@
         <v>1404</v>
       </c>
       <c r="C161" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
@@ -6440,7 +6440,7 @@
         <v>1403</v>
       </c>
       <c r="C162" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
@@ -6448,7 +6448,7 @@
         <v>1402</v>
       </c>
       <c r="C163" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
@@ -6456,7 +6456,7 @@
         <v>1401</v>
       </c>
       <c r="C164" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -6464,7 +6464,7 @@
         <v>1400</v>
       </c>
       <c r="C165" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
@@ -6472,7 +6472,7 @@
         <v>1399</v>
       </c>
       <c r="C166" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
@@ -6480,7 +6480,7 @@
         <v>1398</v>
       </c>
       <c r="C167" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
@@ -6488,7 +6488,7 @@
         <v>1397</v>
       </c>
       <c r="C168" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
@@ -6496,7 +6496,7 @@
         <v>1396</v>
       </c>
       <c r="C169" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
@@ -6504,7 +6504,7 @@
         <v>1395</v>
       </c>
       <c r="C170" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
@@ -6512,7 +6512,7 @@
         <v>1394</v>
       </c>
       <c r="C171" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
@@ -6520,7 +6520,7 @@
         <v>1393</v>
       </c>
       <c r="C172" t="s">
-        <v>1572</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
@@ -6528,7 +6528,7 @@
         <v>1392</v>
       </c>
       <c r="C173" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
@@ -18162,8 +18162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADADFF10-A75D-4336-934E-94B9D3B571F7}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18191,7 +18191,7 @@
       </c>
       <c r="E2">
         <f>COUNTIF(Raw!C:C,D2)</f>
-        <v>98</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -18207,7 +18207,7 @@
       </c>
       <c r="E3">
         <f>COUNTIF(Raw!C:C,D3)</f>
-        <v>1444</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -18223,7 +18223,7 @@
       </c>
       <c r="E4">
         <f>COUNTIF(Raw!C:C,D4)</f>
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Recovered position scoring for extractor.
</commit_message>
<xml_diff>
--- a/tracker/stats.xlsx
+++ b/tracker/stats.xlsx
@@ -2299,7 +2299,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D92" t="inlineStr"/>
@@ -2319,7 +2319,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D93" t="inlineStr"/>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
@@ -2399,7 +2399,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D97" t="inlineStr"/>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D100" t="inlineStr"/>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D101" t="inlineStr"/>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D102" t="inlineStr"/>
@@ -2519,7 +2519,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D103" t="inlineStr"/>
@@ -16815,7 +16815,7 @@
       </c>
       <c r="C817" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D817" t="inlineStr"/>
@@ -16855,7 +16855,7 @@
       </c>
       <c r="C819" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D819" t="inlineStr"/>
@@ -16875,7 +16875,7 @@
       </c>
       <c r="C820" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D820" t="inlineStr"/>
@@ -16895,7 +16895,7 @@
       </c>
       <c r="C821" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D821" t="inlineStr"/>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="C822" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D822" t="inlineStr"/>
@@ -16935,7 +16935,7 @@
       </c>
       <c r="C823" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D823" t="inlineStr"/>
@@ -16955,7 +16955,7 @@
       </c>
       <c r="C824" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D824" t="inlineStr"/>
@@ -16975,7 +16975,7 @@
       </c>
       <c r="C825" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D825" t="inlineStr"/>
@@ -16995,7 +16995,7 @@
       </c>
       <c r="C826" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D826" t="inlineStr"/>
@@ -17015,7 +17015,7 @@
       </c>
       <c r="C827" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D827" t="inlineStr"/>
@@ -17035,7 +17035,7 @@
       </c>
       <c r="C828" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D828" t="inlineStr"/>
@@ -17055,7 +17055,7 @@
       </c>
       <c r="C829" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D829" t="inlineStr"/>
@@ -17075,7 +17075,7 @@
       </c>
       <c r="C830" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D830" t="inlineStr"/>
@@ -17095,7 +17095,7 @@
       </c>
       <c r="C831" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D831" t="inlineStr"/>
@@ -17115,7 +17115,7 @@
       </c>
       <c r="C832" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D832" t="inlineStr"/>
@@ -17155,7 +17155,7 @@
       </c>
       <c r="C834" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D834" t="inlineStr"/>
@@ -17175,7 +17175,7 @@
       </c>
       <c r="C835" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D835" t="inlineStr"/>
@@ -17215,7 +17215,7 @@
       </c>
       <c r="C837" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D837" t="inlineStr"/>
@@ -17255,7 +17255,7 @@
       </c>
       <c r="C839" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D839" t="inlineStr"/>
@@ -17315,7 +17315,7 @@
       </c>
       <c r="C842" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D842" t="inlineStr"/>
@@ -17475,7 +17475,7 @@
       </c>
       <c r="C850" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D850" t="inlineStr"/>
@@ -17495,7 +17495,7 @@
       </c>
       <c r="C851" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D851" t="inlineStr"/>
@@ -17515,7 +17515,7 @@
       </c>
       <c r="C852" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D852" t="inlineStr"/>
@@ -17535,7 +17535,7 @@
       </c>
       <c r="C853" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D853" t="inlineStr"/>
@@ -17555,7 +17555,7 @@
       </c>
       <c r="C854" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D854" t="inlineStr"/>
@@ -17575,7 +17575,7 @@
       </c>
       <c r="C855" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D855" t="inlineStr"/>
@@ -17695,7 +17695,7 @@
       </c>
       <c r="C861" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D861" t="inlineStr"/>
@@ -17715,7 +17715,7 @@
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D862" t="inlineStr"/>
@@ -17735,7 +17735,7 @@
       </c>
       <c r="C863" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D863" t="inlineStr"/>
@@ -17755,7 +17755,7 @@
       </c>
       <c r="C864" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D864" t="inlineStr"/>
@@ -17775,7 +17775,7 @@
       </c>
       <c r="C865" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D865" t="inlineStr"/>
@@ -17795,7 +17795,7 @@
       </c>
       <c r="C866" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D866" t="inlineStr"/>
@@ -17815,7 +17815,7 @@
       </c>
       <c r="C867" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D867" t="inlineStr"/>
@@ -17835,7 +17835,7 @@
       </c>
       <c r="C868" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D868" t="inlineStr"/>
@@ -17855,7 +17855,7 @@
       </c>
       <c r="C869" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D869" t="inlineStr"/>
@@ -17875,7 +17875,7 @@
       </c>
       <c r="C870" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D870" t="inlineStr"/>
@@ -17895,7 +17895,7 @@
       </c>
       <c r="C871" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D871" t="inlineStr"/>
@@ -17915,7 +17915,7 @@
       </c>
       <c r="C872" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D872" t="inlineStr"/>
@@ -17935,7 +17935,7 @@
       </c>
       <c r="C873" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D873" t="inlineStr"/>
@@ -17955,7 +17955,7 @@
       </c>
       <c r="C874" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D874" t="inlineStr"/>
@@ -17975,7 +17975,7 @@
       </c>
       <c r="C875" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D875" t="inlineStr"/>
@@ -17995,7 +17995,7 @@
       </c>
       <c r="C876" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D876" t="inlineStr"/>
@@ -18015,7 +18015,7 @@
       </c>
       <c r="C877" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D877" t="inlineStr"/>
@@ -18035,7 +18035,7 @@
       </c>
       <c r="C878" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D878" t="inlineStr"/>
@@ -18055,7 +18055,7 @@
       </c>
       <c r="C879" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D879" t="inlineStr"/>
@@ -18075,7 +18075,7 @@
       </c>
       <c r="C880" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D880" t="inlineStr"/>
@@ -18095,7 +18095,7 @@
       </c>
       <c r="C881" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D881" t="inlineStr"/>
@@ -18115,7 +18115,7 @@
       </c>
       <c r="C882" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D882" t="inlineStr"/>
@@ -18135,7 +18135,7 @@
       </c>
       <c r="C883" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D883" t="inlineStr"/>
@@ -18155,7 +18155,7 @@
       </c>
       <c r="C884" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D884" t="inlineStr"/>
@@ -18175,7 +18175,7 @@
       </c>
       <c r="C885" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D885" t="inlineStr"/>
@@ -18195,7 +18195,7 @@
       </c>
       <c r="C886" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D886" t="inlineStr"/>
@@ -18215,7 +18215,7 @@
       </c>
       <c r="C887" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D887" t="inlineStr"/>
@@ -18235,7 +18235,7 @@
       </c>
       <c r="C888" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D888" t="inlineStr"/>
@@ -18255,7 +18255,7 @@
       </c>
       <c r="C889" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D889" t="inlineStr"/>
@@ -18275,7 +18275,7 @@
       </c>
       <c r="C890" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D890" t="inlineStr"/>
@@ -18295,7 +18295,7 @@
       </c>
       <c r="C891" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D891" t="inlineStr"/>
@@ -18315,7 +18315,7 @@
       </c>
       <c r="C892" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D892" t="inlineStr"/>
@@ -18335,7 +18335,7 @@
       </c>
       <c r="C893" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D893" t="inlineStr"/>
@@ -18355,7 +18355,7 @@
       </c>
       <c r="C894" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D894" t="inlineStr"/>
@@ -18375,7 +18375,7 @@
       </c>
       <c r="C895" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Incorrect</t>
         </is>
       </c>
       <c r="D895" t="inlineStr"/>
@@ -18395,7 +18395,7 @@
       </c>
       <c r="C896" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D896" t="inlineStr"/>
@@ -18415,7 +18415,7 @@
       </c>
       <c r="C897" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D897" t="inlineStr"/>
@@ -18435,7 +18435,7 @@
       </c>
       <c r="C898" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D898" t="inlineStr"/>
@@ -18455,7 +18455,7 @@
       </c>
       <c r="C899" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Partial</t>
         </is>
       </c>
       <c r="D899" t="inlineStr"/>
@@ -18475,7 +18475,7 @@
       </c>
       <c r="C900" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D900" t="inlineStr"/>
@@ -18495,7 +18495,7 @@
       </c>
       <c r="C901" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D901" t="inlineStr"/>
@@ -18515,7 +18515,7 @@
       </c>
       <c r="C902" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D902" t="inlineStr"/>
@@ -18535,7 +18535,7 @@
       </c>
       <c r="C903" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D903" t="inlineStr"/>
@@ -18555,7 +18555,7 @@
       </c>
       <c r="C904" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D904" t="inlineStr"/>
@@ -18635,7 +18635,7 @@
       </c>
       <c r="C908" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D908" t="inlineStr"/>
@@ -18655,7 +18655,7 @@
       </c>
       <c r="C909" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D909" t="inlineStr"/>
@@ -18675,7 +18675,7 @@
       </c>
       <c r="C910" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D910" t="inlineStr"/>
@@ -18695,7 +18695,7 @@
       </c>
       <c r="C911" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D911" t="inlineStr"/>
@@ -18715,7 +18715,7 @@
       </c>
       <c r="C912" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D912" t="inlineStr"/>
@@ -18735,7 +18735,7 @@
       </c>
       <c r="C913" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D913" t="inlineStr"/>
@@ -18755,7 +18755,7 @@
       </c>
       <c r="C914" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D914" t="inlineStr"/>
@@ -18775,7 +18775,7 @@
       </c>
       <c r="C915" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D915" t="inlineStr"/>
@@ -18795,7 +18795,7 @@
       </c>
       <c r="C916" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D916" t="inlineStr"/>
@@ -18815,7 +18815,7 @@
       </c>
       <c r="C917" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D917" t="inlineStr"/>
@@ -18835,7 +18835,7 @@
       </c>
       <c r="C918" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D918" t="inlineStr"/>
@@ -18855,7 +18855,7 @@
       </c>
       <c r="C919" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D919" t="inlineStr"/>
@@ -18875,7 +18875,7 @@
       </c>
       <c r="C920" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D920" t="inlineStr"/>
@@ -18895,7 +18895,7 @@
       </c>
       <c r="C921" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D921" t="inlineStr"/>
@@ -18915,7 +18915,7 @@
       </c>
       <c r="C922" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D922" t="inlineStr"/>
@@ -18935,7 +18935,7 @@
       </c>
       <c r="C923" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D923" t="inlineStr"/>
@@ -18955,7 +18955,7 @@
       </c>
       <c r="C924" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D924" t="inlineStr"/>
@@ -18975,7 +18975,7 @@
       </c>
       <c r="C925" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D925" t="inlineStr"/>
@@ -19015,7 +19015,7 @@
       </c>
       <c r="C927" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D927" t="inlineStr"/>
@@ -19035,7 +19035,7 @@
       </c>
       <c r="C928" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D928" t="inlineStr"/>
@@ -19055,7 +19055,7 @@
       </c>
       <c r="C929" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D929" t="inlineStr"/>
@@ -19075,7 +19075,7 @@
       </c>
       <c r="C930" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D930" t="inlineStr"/>
@@ -19095,7 +19095,7 @@
       </c>
       <c r="C931" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D931" t="inlineStr"/>
@@ -19115,7 +19115,7 @@
       </c>
       <c r="C932" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D932" t="inlineStr"/>
@@ -19135,7 +19135,7 @@
       </c>
       <c r="C933" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D933" t="inlineStr"/>
@@ -19155,7 +19155,7 @@
       </c>
       <c r="C934" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D934" t="inlineStr"/>
@@ -19175,7 +19175,7 @@
       </c>
       <c r="C935" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D935" t="inlineStr"/>
@@ -19195,7 +19195,7 @@
       </c>
       <c r="C936" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D936" t="inlineStr"/>
@@ -19215,7 +19215,7 @@
       </c>
       <c r="C937" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D937" t="inlineStr"/>
@@ -19235,7 +19235,7 @@
       </c>
       <c r="C938" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D938" t="inlineStr"/>
@@ -19255,7 +19255,7 @@
       </c>
       <c r="C939" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D939" t="inlineStr"/>
@@ -19275,7 +19275,7 @@
       </c>
       <c r="C940" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D940" t="inlineStr"/>
@@ -19295,7 +19295,7 @@
       </c>
       <c r="C941" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D941" t="inlineStr"/>
@@ -19315,7 +19315,7 @@
       </c>
       <c r="C942" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D942" t="inlineStr"/>
@@ -19335,7 +19335,7 @@
       </c>
       <c r="C943" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D943" t="inlineStr"/>
@@ -19355,7 +19355,7 @@
       </c>
       <c r="C944" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D944" t="inlineStr"/>
@@ -19375,7 +19375,7 @@
       </c>
       <c r="C945" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D945" t="inlineStr"/>
@@ -19395,7 +19395,7 @@
       </c>
       <c r="C946" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D946" t="inlineStr"/>
@@ -19415,7 +19415,7 @@
       </c>
       <c r="C947" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D947" t="inlineStr"/>
@@ -19435,7 +19435,7 @@
       </c>
       <c r="C948" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D948" t="inlineStr"/>
@@ -19455,7 +19455,7 @@
       </c>
       <c r="C949" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D949" t="inlineStr"/>
@@ -19475,7 +19475,7 @@
       </c>
       <c r="C950" t="inlineStr">
         <is>
-          <t>Unprocessed</t>
+          <t>Processed</t>
         </is>
       </c>
       <c r="D950" t="inlineStr"/>

</xml_diff>